<commit_message>
LOST CHANGES. Restored some changes and added uncommitted files.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="6660"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="6660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="LOST CHANGES" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$E$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$E$62</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="154">
   <si>
     <t>Email checker TASK: - date range to see last time checked</t>
   </si>
@@ -195,6 +196,291 @@
   </si>
   <si>
     <t>Allow Content for custom controls. For example, Items should have Completed checkbox embedded inside it.</t>
+  </si>
+  <si>
+    <t>Add search for clipboard stuff</t>
+  </si>
+  <si>
+    <t>Is occurances filtering for clipped not working again?</t>
+  </si>
+  <si>
+    <t>Words/phrases dialog needs icon. Same with EditTaskItem</t>
+  </si>
+  <si>
+    <t>On window focused, if a non-taskdash window was focused, bring sub windows to front</t>
+  </si>
+  <si>
+    <t>Left of Links, add a Recency search option</t>
+  </si>
+  <si>
+    <t>Pressing I inserts for FIRST task, not the CURRENT task</t>
+  </si>
+  <si>
+    <t>N and P aren't working</t>
+  </si>
+  <si>
+    <t>Add a Meeting Notes column for next meeting. Or do an overall log feature like I was thinking</t>
+  </si>
+  <si>
+    <t>Add a Quick Reminder feature</t>
+  </si>
+  <si>
+    <t>Change Shift insert keys to be reverse? Shift I more natural for insert?</t>
+  </si>
+  <si>
+    <t>Double click words/phrases copies to clipboard as well, DEFINITELY make it increase occurances</t>
+  </si>
+  <si>
+    <t>Links resizing incorrectly</t>
+  </si>
+  <si>
+    <t>Double click program SalesforceCTI.EXE is doing nothing</t>
+  </si>
+  <si>
+    <t>Open, then double click systray. Spawns new window</t>
+  </si>
+  <si>
+    <t>Keep track of Windows EXEs launched -- add to links? Is that possible?</t>
+  </si>
+  <si>
+    <t>MainWindowViewModel</t>
+  </si>
+  <si>
+    <t>LOST CHANGES - FILES SHOULD STILL EXIST</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>modified:   ../TODO.xlsx</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/ListBoxLinks.xaml.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/bin/Debug/TaskDash.Controls.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/bin/Debug/TaskDash.Controls.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/bin/Debug/TaskDash.Core.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/bin/Debug/TaskDash.Core.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/DesignTimeResolveAssemblyReferencesInput.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/GenerateResource.read.1.tlog</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/GenerateResource.write.1.tlog</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/GeneratedInternalTypeHelper.g.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/ResolveAssemblyReference.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls.csproj.FileListAbsolute.txt</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls_MarkupCompile.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls_MarkupCompile.i.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls_MarkupCompile.i.lref</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Controls/obj/Debug/TaskDash.Controls_MarkupCompile.lref</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/Data/DataManager.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/ModelBase.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/Models/Tasks/Logs.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/Models/Tasks/Task.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/Models/Tasks/Tasks.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/Services/SaveService.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/TaskDash.Core.csproj</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/ViewModelBase.cs</t>
+  </si>
+  <si>
+    <t>deleted:    TaskDash.Core/ViewModels/TaskViewModel.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/bin/Debug/TaskDash.Core.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/bin/Debug/TaskDash.Core.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/obj/Debug/DesignTimeResolveAssemblyReferencesInput.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/obj/Debug/ResolveAssemblyReference.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/obj/Debug/TaskDash.Core.csproj.FileListAbsolute.txt</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/obj/Debug/TaskDash.Core.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.Core/obj/Debug/TaskDash.Core.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.sln</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash.suo</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/AccordianWindow.xaml.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/App.xaml</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/App.xaml.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/DockWindow.xaml.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/MainWindow.xaml</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/MainWindow.xaml.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/Notifications/NotificationManager.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/Properties/Resources.Designer.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/Properties/Resources.resx</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/TaskDash.csproj</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.Controls.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.Controls.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.Core.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.Core.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.exe</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/bin/Debug/TaskDash.pdb</t>
+  </si>
+  <si>
+    <t>deleted:    TaskDash/bin/Debug/TaskDash.vshost.exe.manifest</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/App.g.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/App.g.i.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/DesignTimeResolveAssemblyReferences.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/DesignTimeResolveAssemblyReferencesInput.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/GenerateResource.read.1.tlog</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/GenerateResource.write.1.tlog</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/MainWindow.baml</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/MainWindow.g.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/MainWindow.g.i.cs</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/ResolveAssemblyReference.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash.Properties.Resources.resources</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash.csproj.FileListAbsolute.txt</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash.exe</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash.g.resources</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash_MarkupCompile.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TaskDash_MarkupCompile.i.cache</t>
+  </si>
+  <si>
+    <t>modified:   TaskDash/obj/x86/Debug/TempPE/Properties.Resources.Designer.cs.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstaller/Release/TaskDashInstaller.msi</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstaller/TaskDashInstaller.vdproj</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstallerClasses/bin/Release/TaskDashInstallerClasses.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstallerClasses/bin/Release/TaskDashInstallerClasses.pdb</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstallerClasses/obj/Release/TaskDashInstallerClasses.dll</t>
+  </si>
+  <si>
+    <t>modified:   TaskDashInstallerClasses/obj/Release/TaskDashInstallerClasses.pdb</t>
   </si>
 </sst>
 </file>
@@ -549,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,122 +868,119 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
         <f>A2+(3-B2)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <f>A3+(3-B3)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <f>A4+(3-B4)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
         <f>A5+(3-B5)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <f>A6+(3-B6)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
         <f>A7+(3-B7)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f>A8+(3-B8)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f>A9+(3-B9)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,44 +988,44 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <f>A10+(3-B10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <f>A11+(3-B11)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
         <f>A12+(3-B12)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,95 +1033,89 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>A13+(3-B13)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>A14+(3-B14)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <f>A15+(3-B15)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
         <f>A16+(3-B16)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <f>A17+(3-B17)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
         <f>A18+(3-B18)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -846,74 +1123,74 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <f>A19+(3-B19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <f>A20+(3-B20)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <f>A21+(3-B21)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <f>A22+(3-B22)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23">
         <f>A23+(3-B23)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,59 +1198,59 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <f>A24+(3-B24)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
         <f>A25+(3-B25)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26">
         <f>A26+(3-B26)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <f>A27+(3-B27)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,14 +1258,14 @@
         <v>3</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <f>A28+(3-B28)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -996,62 +1273,66 @@
         <v>3</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <f>A29+(3-B29)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>2</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
         <f>A30+(3-B30)</f>
-        <v>4</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <f>A31+(3-B31)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>2</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <f>A32+(3-B32)</f>
         <v>4</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="2"/>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -1065,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1073,263 +1354,445 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <f>A34+(3-B34)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35">
         <f>A35+(3-B35)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <f>A36+(3-B36)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37">
         <f>A37+(3-B37)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38">
         <f>A38+(3-B38)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
       <c r="C39">
         <f>A39+(3-B39)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <f>A40+(3-B40)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <f>A41+(3-B41)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42">
+      <c r="A42" s="2">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
         <f>A42+(3-B42)</f>
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <f>A43+(3-B43)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
-      </c>
-      <c r="C44">
+      <c r="A44" s="2">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
         <f>A44+(3-B44)</f>
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <f>A45+(3-B45)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <f>A46+(3-B46)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <f>A47+(3-B47)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48">
         <f>A48+(3-B48)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <f>A49+(3-B49)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50">
         <f>A50+(3-B50)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <f>A51+(3-B51)</f>
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <f>A52+(3-B52)</f>
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f>A53+(3-B53)</f>
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <f>A54+(3-B54)</f>
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <f>A55+(3-B55)</f>
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <f>A56+(3-B56)</f>
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <f>A57+(3-B57)</f>
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <f>A58+(3-B58)</f>
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <f>A59+(3-B59)</f>
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <f>A60+(3-B60)</f>
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <f>A61+(3-B61)</f>
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <f>A62+(3-B62)</f>
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E50">
-    <sortState ref="A2:E50">
-      <sortCondition descending="1" ref="C4"/>
+  <autoFilter ref="A1:E62">
+    <sortState ref="A2:E61">
+      <sortCondition descending="1" ref="C3"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:E42">
@@ -1342,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,6 +1833,667 @@
         <v>57</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Still working on logging request dialog. Fixed binding for log entry.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -12,14 +12,14 @@
     <sheet name="LOST CHANGES" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$E$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$E$65</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="158">
   <si>
     <t>Email checker TASK: - date range to see last time checked</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Add a "Location" text box. Such as entering Clay / Rum</t>
+  </si>
+  <si>
+    <t>Switch from NORM driver. Use dependency objects instead of notifychanged. Switch logs to SelectedItem="{Binding Path=SelectedTask.Logs.SelectedLog, Mode=TwoWay}".</t>
   </si>
 </sst>
 </file>
@@ -844,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <f>A8+(3-B8)</f>
+        <f t="shared" ref="C8:C40" si="0">A8+(3-B8)</f>
         <v>9</v>
       </c>
       <c r="D8" t="s">
@@ -987,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f>A9+(3-B9)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D9" t="s">
@@ -1002,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <f>A10+(3-B10)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D10" t="s">
@@ -1020,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <f>A11+(3-B11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D11" t="s">
@@ -1035,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <f>A12+(3-B12)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D12" t="s">
@@ -1050,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <f>A13+(3-B13)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D13" t="s">
@@ -1065,7 +1068,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <f>A14+(3-B14)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D14" t="s">
@@ -1074,17 +1077,17 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <f>A15+(3-B15)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,86 +1098,86 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <f>A16+(3-B16)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <f>A17+(3-B17)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <f>A18+(3-B18)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <f>A19+(3-B19)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <f>A20+(3-B20)</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <f>A21+(3-B21)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1185,11 +1188,11 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <f>A22+(3-B22)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1200,116 +1203,116 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <f>A23+(3-B23)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <f>A24+(3-B24)</f>
-        <v>6</v>
-      </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <f>A25+(3-B25)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <f>A26+(3-B26)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <f>A27+(3-B27)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28">
-        <f>A28+(3-B28)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <f>A29+(3-B29)</f>
-        <v>5</v>
-      </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <f>A30+(3-B30)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,14 +1323,11 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <f>A31+(3-B31)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1338,11 +1338,11 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <f>A32+(3-B32)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -1350,32 +1350,35 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <f>A33+(3-B33)</f>
-        <v>5</v>
-      </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <f>A34+(3-B34)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1386,11 +1389,11 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <f>A35+(3-B35)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,56 +1404,56 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <f>A36+(3-B36)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <f>A37+(3-B37)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <f>A38+(3-B38)</f>
-        <v>4</v>
-      </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <f>A39+(3-B39)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1461,11 +1464,11 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <f>A40+(3-B40)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,11 +1479,11 @@
         <v>2</v>
       </c>
       <c r="C41">
-        <f>A41+(3-B41)</f>
+        <f t="shared" ref="C41:C72" si="1">A41+(3-B41)</f>
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1491,11 +1494,11 @@
         <v>2</v>
       </c>
       <c r="C42">
-        <f>A42+(3-B42)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1506,88 +1509,88 @@
         <v>2</v>
       </c>
       <c r="C43">
-        <f>A43+(3-B43)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>2</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2">
-        <f>A44+(3-B44)</f>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <f>A45+(3-B45)</f>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>2</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2">
-        <f>A46+(3-B46)</f>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <f>A47+(3-B47)</f>
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>9</v>
-      </c>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <f>A48+(3-B48)</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,11 +1601,11 @@
         <v>2</v>
       </c>
       <c r="C49">
-        <f>A49+(3-B49)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,11 +1616,11 @@
         <v>2</v>
       </c>
       <c r="C50">
-        <f>A50+(3-B50)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,11 +1631,11 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <f>A51+(3-B51)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,11 +1646,11 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <f>A52+(3-B52)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,11 +1661,11 @@
         <v>2</v>
       </c>
       <c r="C53">
-        <f>A53+(3-B53)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1670,17 +1673,14 @@
         <v>2</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54">
-        <f>A54+(3-B54)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,26 +1691,29 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <f>A55+(3-B55)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <f>A56+(3-B56)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,11 +1724,11 @@
         <v>2</v>
       </c>
       <c r="C57">
-        <f>A57+(3-B57)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,11 +1739,11 @@
         <v>2</v>
       </c>
       <c r="C58">
-        <f>A58+(3-B58)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,11 +1754,11 @@
         <v>2</v>
       </c>
       <c r="C59">
-        <f>A59+(3-B59)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1763,14 +1766,14 @@
         <v>1</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <f>A60+(3-B60)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1781,11 +1784,11 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <f>A61+(3-B61)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1796,11 +1799,11 @@
         <v>3</v>
       </c>
       <c r="C62">
-        <f>A62+(3-B62)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1811,11 +1814,11 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <f>A63+(3-B63)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1826,15 +1829,30 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <f>A64+(3-B64)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E64">
+  <autoFilter ref="A1:E65">
     <sortState ref="A2:E64">
       <sortCondition descending="1" ref="C2"/>
     </sortState>

</xml_diff>